<commit_message>
added table for address
</commit_message>
<xml_diff>
--- a/DB Design.xlsx
+++ b/DB Design.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="158">
   <si>
     <t>user_dtls</t>
   </si>
@@ -145,15 +145,6 @@
     <t>ROLES_CD</t>
   </si>
   <si>
-    <t>user_addr</t>
-  </si>
-  <si>
-    <t>USER_ADDR_ID</t>
-  </si>
-  <si>
-    <t>PREMISE</t>
-  </si>
-  <si>
     <t>ST_ADDR</t>
   </si>
   <si>
@@ -172,15 +163,6 @@
     <t>VARCHAR(10)</t>
   </si>
   <si>
-    <t>POST_OFFC_ID</t>
-  </si>
-  <si>
-    <t>DISTRCT_ID</t>
-  </si>
-  <si>
-    <t>SUB_DISTRCT_ID</t>
-  </si>
-  <si>
     <t>ADDR_TYPE_CD</t>
   </si>
   <si>
@@ -392,6 +374,123 @@
   </si>
   <si>
     <t>FLAT_MEMBER_TYPE_CD</t>
+  </si>
+  <si>
+    <t>addr_dtls</t>
+  </si>
+  <si>
+    <t>SOCIETY_DTLS_ID</t>
+  </si>
+  <si>
+    <t>society_dtls</t>
+  </si>
+  <si>
+    <t>SOCIETY_NM</t>
+  </si>
+  <si>
+    <t>FILED_BY</t>
+  </si>
+  <si>
+    <t>SOCIETY_ADDR_DTLS_ID</t>
+  </si>
+  <si>
+    <t>SOCIETY_MANAGER_NM</t>
+  </si>
+  <si>
+    <t>SOCIETY_CNTC_NUM</t>
+  </si>
+  <si>
+    <t>SOCIETY_CHAIRMAN_NM</t>
+  </si>
+  <si>
+    <t>SOCIETY_CHAIRMAN_CNTC_NUM</t>
+  </si>
+  <si>
+    <t>SOCIETY_SECTRETARY_NM</t>
+  </si>
+  <si>
+    <t>SOCIETY_SECTRETARY_CNTC_NUM</t>
+  </si>
+  <si>
+    <t>SOCIETY_TREASURER_NM</t>
+  </si>
+  <si>
+    <t>SOCIETY_TREASURER_CNTC_NUM</t>
+  </si>
+  <si>
+    <t>TWO_BHK_COUNT</t>
+  </si>
+  <si>
+    <t>ONE_BHK_COUNT</t>
+  </si>
+  <si>
+    <t>THREE_BHK_N_ABV_COUNT</t>
+  </si>
+  <si>
+    <t>BUNGLOWS_COUNT</t>
+  </si>
+  <si>
+    <t>TOTAL_UNITS</t>
+  </si>
+  <si>
+    <t>IS_SOCIETY_REG_WT_DEPT_OF_COOP_SOCIETY</t>
+  </si>
+  <si>
+    <t>IS_SOCIETY_REG_WT_FED_OF_COOP_SOCIETY</t>
+  </si>
+  <si>
+    <t>REG_WT_DEPT_OF_COOP_SOCIETY_SINCE</t>
+  </si>
+  <si>
+    <t>FED_WT_DEPT_OF_COOP_SOCIETY_SINCE</t>
+  </si>
+  <si>
+    <t>society_facilities_dtls</t>
+  </si>
+  <si>
+    <t>SOCIETY_FACILITIES_DTLS_ID</t>
+  </si>
+  <si>
+    <t>FACILITY_ID</t>
+  </si>
+  <si>
+    <t>facility_dtls</t>
+  </si>
+  <si>
+    <t>FACILITY_NM</t>
+  </si>
+  <si>
+    <t>VARCHAR(150)</t>
+  </si>
+  <si>
+    <t>AVG_MONTHLY_ELEC_BILL</t>
+  </si>
+  <si>
+    <t>TOTAL__MONTHLY_MAINT_CHRGS_COLLECTED</t>
+  </si>
+  <si>
+    <t>IS_ADQ_CCTVS_INST</t>
+  </si>
+  <si>
+    <t>IS_LIGHT_REQ</t>
+  </si>
+  <si>
+    <t>SW_USED_NM</t>
+  </si>
+  <si>
+    <t>NO_OF_SEC_GUARDS_PER_SHIFTS</t>
+  </si>
+  <si>
+    <t>NO_OF_SOCIETY_STAFF</t>
+  </si>
+  <si>
+    <t>VARCHAR(500)</t>
+  </si>
+  <si>
+    <t>ROW_HOUSE_COUNT</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
   </si>
 </sst>
 </file>
@@ -415,7 +514,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +524,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -514,6 +619,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,10 +644,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:K87"/>
+  <dimension ref="A3:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -876,21 +982,21 @@
     <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:11">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="I3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="I3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
@@ -902,16 +1008,16 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
       <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>10</v>
@@ -936,14 +1042,12 @@
       <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -954,12 +1058,14 @@
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2" t="s">
-        <v>4</v>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
@@ -978,18 +1084,20 @@
         <v>28</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>6</v>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1002,17 +1110,17 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1023,14 +1131,12 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>8</v>
@@ -1050,19 +1156,21 @@
       <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>49</v>
+      <c r="J10" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1075,19 +1183,17 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1100,19 +1206,17 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1125,19 +1229,17 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1150,19 +1252,10 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1174,18 +1267,11 @@
         <v>19</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="3" t="s">
-        <v>20</v>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1198,18 +1284,16 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="I16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1"/>
@@ -1221,17 +1305,19 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1244,14 +1330,16 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="3" t="s">
-        <v>24</v>
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>3</v>
@@ -1266,6 +1354,22 @@
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1276,6 +1380,15 @@
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="I20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1"/>
@@ -1285,16 +1398,13 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-      <c r="I21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1"/>
@@ -1304,23 +1414,17 @@
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>56</v>
+      <c r="E22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1331,18 +1435,18 @@
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>3</v>
@@ -1351,62 +1455,42 @@
     <row r="24" spans="1:11">
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="E25" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="E26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="G26" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1414,25 +1498,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="3" t="s">
-        <v>20</v>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
@@ -1446,17 +1530,19 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="3" t="s">
-        <v>23</v>
+      <c r="I28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1464,24 +1550,26 @@
         <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1489,17 +1577,26 @@
         <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1510,6 +1607,20 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1"/>
@@ -1519,11 +1630,13 @@
       <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1"/>
@@ -1533,19 +1646,12 @@
       <c r="C33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="I33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>61</v>
+      <c r="I33" s="1"/>
+      <c r="J33" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1556,42 +1662,27 @@
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>2</v>
+      <c r="E34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="E35" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1600,65 +1691,60 @@
         <v>8</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
+      <c r="A37" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
       <c r="E37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="I37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="3" t="s">
-        <v>20</v>
+      <c r="E38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1666,87 +1752,112 @@
         <v>8</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="3" t="s">
-        <v>24</v>
+      <c r="I39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>72</v>
+      <c r="B40" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A41" s="1"/>
       <c r="B41" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1"/>
       <c r="B42" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1"/>
-      <c r="B43" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="1"/>
+      <c r="B43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I43" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>10</v>
@@ -1755,946 +1866,1325 @@
     <row r="44" spans="1:11">
       <c r="A44" s="1"/>
       <c r="B44" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="I44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>10</v>
+      <c r="I44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1"/>
       <c r="B45" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1"/>
       <c r="B46" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="F46" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I46" s="1"/>
-      <c r="J46" s="1" t="s">
-        <v>86</v>
+      <c r="J46" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I47" s="1"/>
-      <c r="J47" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="E48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="E49" s="1"/>
-      <c r="F49" s="3" t="s">
-        <v>20</v>
+      <c r="A49" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="E49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="J49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="F50" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I51" s="1"/>
-      <c r="J51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K51" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="A52" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I52" s="1"/>
-      <c r="J52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I53" s="1"/>
-      <c r="J53" s="3" t="s">
-        <v>23</v>
+      <c r="G53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I54" s="1"/>
-      <c r="J54" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="I55" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K55" s="14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>10</v>
+      <c r="E56" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I57" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>87</v>
+      <c r="B58" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="1"/>
       <c r="B59" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I59" s="1" t="s">
+      <c r="E59" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K59" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K59" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="1"/>
       <c r="B60" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K60" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="1"/>
       <c r="B61" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K61" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="1"/>
-      <c r="B62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="I62" s="1"/>
-      <c r="J62" s="1" t="s">
-        <v>117</v>
+      <c r="J62" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="E63" s="1"/>
-      <c r="F63" s="4" t="s">
-        <v>92</v>
+      <c r="F63" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="I63" s="1"/>
-      <c r="J63" s="1" t="s">
-        <v>118</v>
+      <c r="J63" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:11">
-      <c r="E64" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A64" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="E64" s="1"/>
       <c r="F64" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>10</v>
+        <v>43</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
+      <c r="A65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>10</v>
+      <c r="I65" s="1"/>
+      <c r="J65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F66" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I66" s="1"/>
-      <c r="J66" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I67" s="1"/>
-      <c r="J67" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K67" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I68" s="1"/>
-      <c r="J68" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="E69" s="1"/>
-      <c r="F69" s="3" t="s">
-        <v>20</v>
+      <c r="F69" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I69" s="1"/>
-      <c r="J69" s="3" t="s">
-        <v>23</v>
+        <v>85</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I70" s="1"/>
-      <c r="J70" s="3" t="s">
-        <v>24</v>
+      <c r="J70" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="1"/>
-      <c r="B71" s="1" t="s">
-        <v>108</v>
+      <c r="B71" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="1"/>
       <c r="B72" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="I72" s="1"/>
+      <c r="J72" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="1"/>
       <c r="B73" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="F73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I73" s="1"/>
+      <c r="J73" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="1"/>
       <c r="B74" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I74" s="1"/>
+      <c r="J74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="I75" s="1"/>
+      <c r="J75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="E76" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I74" s="1" t="s">
+      <c r="K76" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="30">
+      <c r="A77" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11">
-      <c r="A75" s="1"/>
-      <c r="B75" s="3" t="s">
+      <c r="B77" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I77" s="1"/>
+      <c r="J77" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K75" s="1" t="s">
+      <c r="K77" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
-      <c r="E76" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J76" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
-      <c r="A77" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="E77" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I77" s="1"/>
-      <c r="J77" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K77" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A78" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I78" s="1"/>
-      <c r="J78" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K78" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
-      <c r="A79" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C79" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I79" s="1"/>
-      <c r="J79" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I80" s="1"/>
-      <c r="J80" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="I80" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I81" s="1"/>
-      <c r="J81" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E82" s="1"/>
-      <c r="F82" s="4" t="s">
-        <v>97</v>
+      <c r="F82" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I82" s="1"/>
-      <c r="J82" s="3" t="s">
-        <v>24</v>
+      <c r="J82" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>3</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="1"/>
-      <c r="B83" s="1" t="s">
-        <v>97</v>
+      <c r="B83" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K83" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="1"/>
       <c r="B84" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E84" s="1"/>
-      <c r="F84" s="3" t="s">
-        <v>20</v>
+      <c r="F84" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="1"/>
       <c r="B85" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="1"/>
       <c r="B86" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="1"/>
-      <c r="B87" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E87" s="1"/>
       <c r="F87" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="E88" s="1"/>
+      <c r="F88" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="G88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="1"/>
+      <c r="B93" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="1"/>
+      <c r="B94" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="1"/>
+      <c r="B95" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="1"/>
+      <c r="B96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="5:11">
+      <c r="E97" s="1"/>
+      <c r="F97" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="5:11">
+      <c r="E98" s="1"/>
+      <c r="F98" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="5:11">
+      <c r="E99" s="1"/>
+      <c r="F99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="5:11">
+      <c r="I100" s="1"/>
+      <c r="J100" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="5:11">
+      <c r="I101" s="1"/>
+      <c r="J101" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="5:11">
+      <c r="I102" s="1"/>
+      <c r="J102" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="5:11">
+      <c r="I103" s="1"/>
+      <c r="J103" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="5:11">
+      <c r="I104" s="1"/>
+      <c r="J104" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="5:11">
+      <c r="I105" s="1"/>
+      <c r="J105" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="5:11">
+      <c r="I106" s="1"/>
+      <c r="J106" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="5:11">
+      <c r="I107" s="1"/>
+      <c r="J107" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="5:11">
+      <c r="I108" s="1"/>
+      <c r="J108" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="5:11">
+      <c r="I109" s="1"/>
+      <c r="J109" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="5:11">
+      <c r="I110" s="1"/>
+      <c r="J110" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="5:11">
+      <c r="I111" s="1"/>
+      <c r="J111" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="5:11">
+      <c r="I112" s="1"/>
+      <c r="J112" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="9:11">
+      <c r="I113" s="1"/>
+      <c r="J113" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="9:11">
+      <c r="I114" s="1"/>
+      <c r="J114" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K114" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="I73:K73"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I57:K57"/>
+  <mergeCells count="21">
+    <mergeCell ref="I80:K80"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I52:K52"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E22:G22"/>
     <mergeCell ref="A37:C37"/>
-    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
     <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>